<commit_message>
Change the local path for 0.3% HF to server path.
</commit_message>
<xml_diff>
--- a/main/classifyPillars.xlsx
+++ b/main/classifyPillars.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12105" tabRatio="620" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trainingData" sheetId="6" r:id="rId1"/>
@@ -932,184 +932,184 @@
     <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy1.00%HF/06/20kX _13578.dm3</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13243.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13244.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13245.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13246.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13247.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13248.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13249.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13250.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13251.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13252.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13253.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/00/20kX _13254.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13819.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13820.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13821.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13822.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13823.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13824.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13825.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13826.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13827.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13828.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13829.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/01/20kX _13830.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13831.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13832.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13833.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13834.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13835.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13836.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13837.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13838.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13839.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13840.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13841.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/02/20kX _13842.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13843.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13844.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13845.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13846.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13847.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13848.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13849.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13850.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13851.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13852.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13853.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/03/20kX _13854.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13855.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13856.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13857.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13858.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13859.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13860.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13861.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13862.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13863.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13864.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13865.dm3</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/exSitu/RestoreBy0.30%HF/04/20kX _13866.dm3</t>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13243.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13244.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13245.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13246.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13247.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13248.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13249.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13250.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13251.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13252.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13253.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/00/20kX _13254.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13819.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13820.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13821.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13822.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13823.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13824.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13825.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13826.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13827.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13828.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13829.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/01/20kX _13830.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13831.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13832.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13833.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13834.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13835.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13836.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13837.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13838.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13839.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13840.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13841.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/02/20kX _13842.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13843.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13844.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13845.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13846.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13847.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13848.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13849.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13850.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13851.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13852.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13853.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/03/20kX _13854.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13855.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13856.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13857.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13858.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13859.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13860.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13861.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13862.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13863.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13864.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13865.dm3</t>
+  </si>
+  <si>
+    <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.30%HF/04/20kX _13866.dm3</t>
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/RestorePillars/exSitu/RestoreBy0.10%HF/00/20kX _13243.dm3</t>
@@ -1486,10 +1486,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1504,17 +1504,38 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1526,7 +1547,60 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1541,75 +1615,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1622,8 +1628,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1637,24 +1652,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1669,13 +1669,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1687,19 +1681,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1711,25 +1711,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1747,7 +1747,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1759,19 +1831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1783,73 +1843,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1895,8 +1895,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1917,17 +1919,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1941,13 +1937,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1978,138 +1978,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2450,7 +2450,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3911,9 +3911,9 @@
   <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50:K51"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6914,9 +6914,9 @@
   <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:K29"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -9917,9 +9917,9 @@
   <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:K66"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -12922,7 +12922,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -15095,9 +15095,9 @@
   <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>

</xml_diff>